<commit_message>
last pipeline step and results
</commit_message>
<xml_diff>
--- a/TestResults.xlsx
+++ b/TestResults.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johan\Documents\GitHub\BERT_ROC\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAADB07-36C4-41F3-BBCB-3F17CFB20225}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,42 +25,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
-  <si>
-    <t xml:space="preserve">Model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hyp-Only</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Noise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Negated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TriggerOnly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TriggerRemoved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TriggerSynonymized</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Translated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BERT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choice</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Hyp-Only</t>
+  </si>
+  <si>
+    <t>Noise</t>
+  </si>
+  <si>
+    <t>Negated</t>
+  </si>
+  <si>
+    <t>TriggerOnly</t>
+  </si>
+  <si>
+    <t>TriggerRemoved</t>
+  </si>
+  <si>
+    <t>TriggerSynonymized</t>
+  </si>
+  <si>
+    <t>Translated</t>
+  </si>
+  <si>
+    <t>BERT</t>
+  </si>
+  <si>
+    <t>Choice</t>
   </si>
   <si>
     <t xml:space="preserve">              precision    recall  f1-score   support
@@ -82,7 +87,7 @@
 weighted avg       0.58      0.57      0.58       174</t>
   </si>
   <si>
-    <t xml:space="preserve">Binary</t>
+    <t>Binary</t>
   </si>
   <si>
     <t xml:space="preserve">              precision    recall  f1-score   support
@@ -109,7 +114,7 @@
 weighted avg       0.54      0.52      0.45       348</t>
   </si>
   <si>
-    <t xml:space="preserve">RocOnly</t>
+    <t>RocOnly</t>
   </si>
   <si>
     <t xml:space="preserve">              precision    recall  f1-score   support
@@ -152,7 +157,7 @@
 weighted avg       0.33      0.44      0.33       348</t>
   </si>
   <si>
-    <t xml:space="preserve">ClozeOnly</t>
+    <t>ClozeOnly</t>
   </si>
   <si>
     <t xml:space="preserve">              precision    recall  f1-score   support
@@ -203,7 +208,7 @@
 weighted avg       0.83      0.83      0.83       348</t>
   </si>
   <si>
-    <t xml:space="preserve">RocCloze</t>
+    <t>RocCloze</t>
   </si>
   <si>
     <t xml:space="preserve">              precision    recall  f1-score   support
@@ -246,7 +251,7 @@
 weighted avg       0.86      0.86      0.86       348</t>
   </si>
   <si>
-    <t xml:space="preserve">Cloze+5000Roc</t>
+    <t>Cloze+5000Roc</t>
   </si>
   <si>
     <t xml:space="preserve">              precision    recall  f1-score   support
@@ -288,15 +293,15 @@
    macro avg       0.84      0.84      0.84       348
 weighted avg       0.84      0.84      0.84       348</t>
   </si>
+  <si>
+    <t>Hard Testset</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -305,22 +310,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -334,6 +324,13 @@
       <family val="3"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -344,107 +341,83 @@
     </fill>
   </fills>
   <borders count="4">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
-      <right style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
-      <right style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+  <cellStyles count="1">
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
@@ -460,11 +433,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Grafik 5" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
+        <xdr:cNvPr id="2" name="Grafik 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -497,11 +476,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Grafik 6" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
+        <xdr:cNvPr id="3" name="Grafik 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -534,11 +519,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Grafik 7" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId3"/>
+        <xdr:cNvPr id="4" name="Grafik 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -571,11 +562,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Grafik 9" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId4"/>
+        <xdr:cNvPr id="5" name="Grafik 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -608,11 +605,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Grafik 10" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId5"/>
+        <xdr:cNvPr id="6" name="Grafik 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -645,11 +648,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Grafik 11" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId6"/>
+        <xdr:cNvPr id="7" name="Grafik 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -682,11 +691,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Grafik 12" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId7"/>
+        <xdr:cNvPr id="8" name="Grafik 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -719,11 +734,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Grafik 13" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId8"/>
+        <xdr:cNvPr id="9" name="Grafik 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -756,11 +777,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Grafik 14" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId9"/>
+        <xdr:cNvPr id="10" name="Grafik 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -793,11 +820,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Grafik 15" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId10"/>
+        <xdr:cNvPr id="11" name="Grafik 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -830,11 +863,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Grafik 16" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId11"/>
+        <xdr:cNvPr id="12" name="Grafik 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -867,11 +906,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Grafik 17" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId12"/>
+        <xdr:cNvPr id="13" name="Grafik 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -904,11 +949,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Grafik 18" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId13"/>
+        <xdr:cNvPr id="14" name="Grafik 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -941,11 +992,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Grafik 19" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId14"/>
+        <xdr:cNvPr id="15" name="Grafik 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -978,11 +1035,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Grafik 20" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId15"/>
+        <xdr:cNvPr id="16" name="Grafik 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1015,11 +1078,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Grafik 21" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId16"/>
+        <xdr:cNvPr id="17" name="Grafik 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1052,11 +1121,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Grafik 22" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId17"/>
+        <xdr:cNvPr id="18" name="Grafik 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1089,11 +1164,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Grafik 23" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId18"/>
+        <xdr:cNvPr id="19" name="Grafik 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1126,11 +1207,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Grafik 24" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId19"/>
+        <xdr:cNvPr id="20" name="Grafik 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1163,11 +1250,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Grafik 25" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId20"/>
+        <xdr:cNvPr id="21" name="Grafik 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1200,11 +1293,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Grafik 26" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId21"/>
+        <xdr:cNvPr id="22" name="Grafik 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1237,11 +1336,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Grafik 27" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId22"/>
+        <xdr:cNvPr id="23" name="Grafik 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1274,11 +1379,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="Grafik 28" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId23"/>
+        <xdr:cNvPr id="24" name="Grafik 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1306,16 +1417,22 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>3373920</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>1115280</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Grafik 29" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId24"/>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>855</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Grafik 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1348,11 +1465,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="Grafik 30" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId25"/>
+        <xdr:cNvPr id="26" name="Grafik 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1385,11 +1508,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="Grafik 31" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId26"/>
+        <xdr:cNvPr id="27" name="Grafik 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1422,11 +1551,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="Grafik 32" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId27"/>
+        <xdr:cNvPr id="28" name="Grafik 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1459,11 +1594,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="27" name="Grafik 33" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId28"/>
+        <xdr:cNvPr id="29" name="Grafik 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1496,11 +1637,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="Grafik 34" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId29"/>
+        <xdr:cNvPr id="30" name="Grafik 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1533,11 +1680,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="29" name="Grafik 35" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId30"/>
+        <xdr:cNvPr id="31" name="Grafik 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1570,11 +1723,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="30" name="Grafik 36" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId31"/>
+        <xdr:cNvPr id="32" name="Grafik 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1607,11 +1766,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="31" name="Grafik 37" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId32"/>
+        <xdr:cNvPr id="33" name="Grafik 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1644,11 +1809,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="32" name="Grafik 38" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId33"/>
+        <xdr:cNvPr id="34" name="Grafik 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1681,11 +1852,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="33" name="Grafik 39" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId34"/>
+        <xdr:cNvPr id="35" name="Grafik 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1718,11 +1895,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="34" name="Grafik 40" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId35"/>
+        <xdr:cNvPr id="36" name="Grafik 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1755,11 +1938,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="35" name="Grafik 41" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId36"/>
+        <xdr:cNvPr id="37" name="Grafik 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1792,11 +1981,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="36" name="Grafik 42" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId37"/>
+        <xdr:cNvPr id="38" name="Grafik 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1829,11 +2024,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="37" name="Grafik 43" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId38"/>
+        <xdr:cNvPr id="39" name="Grafik 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1860,17 +2061,23 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>3387960</xdr:colOff>
+      <xdr:colOff>3378435</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>1085040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="38" name="Grafik 44" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId39"/>
+        <xdr:cNvPr id="40" name="Grafik 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1903,11 +2110,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="39" name="Grafik 45" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId40"/>
+        <xdr:cNvPr id="41" name="Grafik 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1940,11 +2153,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="40" name="Grafik 46" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId41"/>
+        <xdr:cNvPr id="42" name="Grafik 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1977,11 +2196,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="41" name="Grafik 47" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId42"/>
+        <xdr:cNvPr id="43" name="Grafik 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -2014,11 +2239,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="42" name="Grafik 48" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId43"/>
+        <xdr:cNvPr id="44" name="Grafik 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -2051,11 +2282,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="43" name="Grafik 49" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId44"/>
+        <xdr:cNvPr id="45" name="Grafik 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -2069,6 +2306,446 @@
         <a:ln>
           <a:noFill/>
         </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>161926</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>3343276</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1103663</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="46" name="Grafik 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B281ACCD-B8A6-4326-AFFB-C1AD1A2F61BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="28946476" y="228601"/>
+          <a:ext cx="3181350" cy="1065562"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>3362325</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1077160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="Grafik 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A44AD65-E63A-4F93-A7EA-FC8AFA363527}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="28898850" y="1343025"/>
+          <a:ext cx="3248025" cy="1039060"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>3355976</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1085850</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="49" name="Grafik 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC7F26FE-405F-4EB2-B320-116E7CCF01F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="28927425" y="3571875"/>
+          <a:ext cx="3213101" cy="1047750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>3371850</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1092855</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="50" name="Grafik 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34D5ED69-C74F-4120-BB20-C15684BA2D5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="28908375" y="2447925"/>
+          <a:ext cx="3248025" cy="1064280"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>3346215</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1104900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="51" name="Grafik 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{629D6AB5-F3BC-42E0-8A8D-69849F7A9CD5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="28822650" y="5791200"/>
+          <a:ext cx="3308115" cy="1076325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>133351</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>3352800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1080937</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="52" name="Grafik 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA8883EA-A1FC-42AF-BDDA-997D529C00C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="28917901" y="4676775"/>
+          <a:ext cx="3219449" cy="1052362"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>3314700</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1058603</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="53" name="Grafik 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96C1F652-DE32-4443-A73F-1FC13989FDAA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="28965525" y="8010525"/>
+          <a:ext cx="3133725" cy="1039553"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>66676</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>3400774</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="54" name="Grafik 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C726195E-A08D-4B08-A810-CFF97D0FBFF0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="28851226" y="6896100"/>
+          <a:ext cx="3334098" cy="1095375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>3381375</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>730</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="55" name="Grafik 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7609734B-9ACB-43E6-A680-19FC28C0554D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="28784550" y="10248900"/>
+          <a:ext cx="3381375" cy="1086580"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>3388891</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1076325</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="56" name="Grafik 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E5690FA-AB7F-408E-8797-DD614B4B38FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="28784550" y="9296400"/>
+          <a:ext cx="3388891" cy="885825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -2076,65 +2753,359 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="0" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="I11" activeCellId="0" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="3" style="0" width="50.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="11" style="0" width="24.57"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="3" max="10" width="50.7109375" customWidth="1"/>
+    <col min="11" max="11" width="51.28515625" customWidth="1"/>
+    <col min="12" max="15" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
+      <c r="K1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="87.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:15" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2151,8 +3122,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="87.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4"/>
+    <row r="3" spans="1:15" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
       <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
@@ -2167,8 +3138,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="87.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:15" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -2185,8 +3156,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="87.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4"/>
+    <row r="5" spans="1:15" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
       <c r="B5" s="5" t="s">
         <v>15</v>
       </c>
@@ -2201,8 +3172,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="87.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:15" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -2219,8 +3190,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="87.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4"/>
+    <row r="7" spans="1:15" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
       <c r="B7" s="5" t="s">
         <v>15</v>
       </c>
@@ -2235,8 +3206,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="87.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:15" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -2253,8 +3224,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="87.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4"/>
+    <row r="9" spans="1:15" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
       <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
@@ -2269,8 +3240,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="87.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:15" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -2286,8 +3257,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="87.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4"/>
+    <row r="11" spans="1:15" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
       <c r="B11" s="5" t="s">
         <v>15</v>
       </c>
@@ -2309,13 +3280,8 @@
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A10:A11"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
corrected entry in Noise column
</commit_message>
<xml_diff>
--- a/TestResults.xlsx
+++ b/TestResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johan\Documents\GitHub\BERT_ROC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAADB07-36C4-41F3-BBCB-3F17CFB20225}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3E6833-55F9-4852-8AD3-C7A1853DDCC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -383,9 +383,6 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -399,6 +396,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1324,49 +1324,6 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>68040</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>27360</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>3296160</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1084680</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Grafik 27">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11394360" y="1316880"/>
-          <a:ext cx="3228120" cy="1057320"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
       <xdr:colOff>70200</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>21240</xdr:rowOff>
@@ -1389,7 +1346,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1432,7 +1389,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1475,7 +1432,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1518,7 +1475,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1561,7 +1518,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1604,7 +1561,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1647,7 +1604,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1690,7 +1647,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1733,7 +1690,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1776,7 +1733,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1819,7 +1776,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1862,7 +1819,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1905,7 +1862,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1948,7 +1905,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1991,7 +1948,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -2034,7 +1991,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -2077,7 +2034,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -2120,7 +2077,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -2163,7 +2120,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -2206,7 +2163,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -2337,6 +2294,50 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="28946476" y="228601"/>
+          <a:ext cx="3181350" cy="1065562"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>3362325</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1077160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="Grafik 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A44AD65-E63A-4F93-A7EA-FC8AFA363527}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42"/>
         <a:stretch>
           <a:fillRect/>
@@ -2344,8 +2345,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28946476" y="228601"/>
-          <a:ext cx="3181350" cy="1065562"/>
+          <a:off x="28898850" y="1343025"/>
+          <a:ext cx="3248025" cy="1039060"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2357,22 +2358,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>3362325</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1077160</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="48" name="Grafik 47">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A44AD65-E63A-4F93-A7EA-FC8AFA363527}"/>
+      <xdr:colOff>3355976</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1085850</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="49" name="Grafik 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC7F26FE-405F-4EB2-B320-116E7CCF01F5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2388,8 +2389,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28898850" y="1343025"/>
-          <a:ext cx="3248025" cy="1039060"/>
+          <a:off x="28927425" y="3571875"/>
+          <a:ext cx="3213101" cy="1047750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2401,22 +2402,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>3355976</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>1085850</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="49" name="Grafik 48">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC7F26FE-405F-4EB2-B320-116E7CCF01F5}"/>
+      <xdr:colOff>3371850</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1092855</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="50" name="Grafik 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34D5ED69-C74F-4120-BB20-C15684BA2D5C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2432,8 +2433,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28927425" y="3571875"/>
-          <a:ext cx="3213101" cy="1047750"/>
+          <a:off x="28908375" y="2447925"/>
+          <a:ext cx="3248025" cy="1064280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2445,22 +2446,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>3371850</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>1092855</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="50" name="Grafik 49">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34D5ED69-C74F-4120-BB20-C15684BA2D5C}"/>
+      <xdr:colOff>3346215</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1104900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="51" name="Grafik 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{629D6AB5-F3BC-42E0-8A8D-69849F7A9CD5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2476,8 +2477,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28908375" y="2447925"/>
-          <a:ext cx="3248025" cy="1064280"/>
+          <a:off x="28822650" y="5791200"/>
+          <a:ext cx="3308115" cy="1076325"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2489,22 +2490,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:colOff>133351</xdr:colOff>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>3346215</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>1104900</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="51" name="Grafik 50">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{629D6AB5-F3BC-42E0-8A8D-69849F7A9CD5}"/>
+      <xdr:colOff>3352800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1080937</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="52" name="Grafik 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA8883EA-A1FC-42AF-BDDA-997D529C00C1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2520,8 +2521,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28822650" y="5791200"/>
-          <a:ext cx="3308115" cy="1076325"/>
+          <a:off x="28917901" y="4676775"/>
+          <a:ext cx="3219449" cy="1052362"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2533,22 +2534,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>133351</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>3352800</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>1080937</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="52" name="Grafik 51">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA8883EA-A1FC-42AF-BDDA-997D529C00C1}"/>
+      <xdr:colOff>3314700</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1058603</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="53" name="Grafik 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96C1F652-DE32-4443-A73F-1FC13989FDAA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2564,8 +2565,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28917901" y="4676775"/>
-          <a:ext cx="3219449" cy="1052362"/>
+          <a:off x="28965525" y="8010525"/>
+          <a:ext cx="3133725" cy="1039553"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2577,22 +2578,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
+      <xdr:colOff>66676</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>3400774</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>3314700</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>1058603</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="53" name="Grafik 52">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96C1F652-DE32-4443-A73F-1FC13989FDAA}"/>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="54" name="Grafik 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C726195E-A08D-4B08-A810-CFF97D0FBFF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2608,8 +2609,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28965525" y="8010525"/>
-          <a:ext cx="3133725" cy="1039553"/>
+          <a:off x="28851226" y="6896100"/>
+          <a:ext cx="3334098" cy="1095375"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2621,22 +2622,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>66676</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>3400774</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="54" name="Grafik 53">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C726195E-A08D-4B08-A810-CFF97D0FBFF0}"/>
+      <xdr:colOff>3381375</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>730</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="55" name="Grafik 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7609734B-9ACB-43E6-A680-19FC28C0554D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2652,8 +2653,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28851226" y="6896100"/>
-          <a:ext cx="3334098" cy="1095375"/>
+          <a:off x="28784550" y="10248900"/>
+          <a:ext cx="3381375" cy="1086580"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2666,21 +2667,21 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>3381375</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>730</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="55" name="Grafik 54">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7609734B-9ACB-43E6-A680-19FC28C0554D}"/>
+      <xdr:colOff>3388891</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1076325</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="56" name="Grafik 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E5690FA-AB7F-408E-8797-DD614B4B38FD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2696,35 +2697,35 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28784550" y="10248900"/>
-          <a:ext cx="3381375" cy="1086580"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
+          <a:off x="28784550" y="9296400"/>
+          <a:ext cx="3388891" cy="885825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>666257</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>3388891</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>1076325</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="56" name="Grafik 55">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E5690FA-AB7F-408E-8797-DD614B4B38FD}"/>
+      <xdr:rowOff>161765</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="Grafik 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AD8DD11-50DA-497A-9B3B-B27FFBB9B5B7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2740,8 +2741,96 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28784550" y="9296400"/>
-          <a:ext cx="3388891" cy="885825"/>
+          <a:off x="32204025" y="7991475"/>
+          <a:ext cx="3942857" cy="1276190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>818657</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>314165</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="57" name="Grafik 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{447E6B5B-ACFD-4DA6-9E66-FF0C6A22998E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="32356425" y="8143875"/>
+          <a:ext cx="3942857" cy="1276190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3293376</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1076325</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="59" name="Grafik 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2837B3A5-E745-4362-8C22-F050E6C4F9E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8582025" y="1343025"/>
+          <a:ext cx="3207651" cy="1038225"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3052,9 +3141,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3066,209 +3155,209 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
     </row>
     <row r="2" spans="1:15" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="G2" s="7" t="s">
+      <c r="C2" s="5"/>
+      <c r="G2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="G3" s="7" t="s">
+      <c r="C3" s="5"/>
+      <c r="G3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="G4" s="7" t="s">
+      <c r="C4" s="5"/>
+      <c r="G4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="G5" s="7" t="s">
+      <c r="C5" s="5"/>
+      <c r="G5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="G6" s="7" t="s">
+      <c r="C6" s="5"/>
+      <c r="G6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="G7" s="7" t="s">
+      <c r="C7" s="5"/>
+      <c r="G7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="G8" s="7" t="s">
+      <c r="C8" s="5"/>
+      <c r="G8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="8"/>
+      <c r="B9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="G9" s="7" t="s">
+      <c r="C9" s="5"/>
+      <c r="G9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="8"/>
+      <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="6" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
default performance on first 100 samples
</commit_message>
<xml_diff>
--- a/TestResults.xlsx
+++ b/TestResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johan\Documents\GitHub\BERT_ROC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3E6833-55F9-4852-8AD3-C7A1853DDCC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE67C206-67F1-42CE-9D48-EE713C6A48AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="3945" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
   <si>
     <t>Model</t>
   </si>
@@ -295,6 +295,9 @@
   </si>
   <si>
     <t>Hard Testset</t>
+  </si>
+  <si>
+    <t>Default first 100</t>
   </si>
 </sst>
 </file>
@@ -1324,15 +1327,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>70200</xdr:colOff>
+      <xdr:colOff>60675</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>21240</xdr:rowOff>
+      <xdr:rowOff>30765</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3317760</xdr:colOff>
+      <xdr:colOff>3308235</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1074960</xdr:rowOff>
+      <xdr:rowOff>1084485</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1351,7 +1354,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11396520" y="196200"/>
+          <a:off x="8556975" y="221265"/>
           <a:ext cx="3247560" cy="1053720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1437,7 +1440,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11435040" y="2458440"/>
+          <a:off x="8605020" y="2473710"/>
           <a:ext cx="3183840" cy="1050840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2709,23 +2712,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>666257</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>161765</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="47" name="Grafik 46">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AD8DD11-50DA-497A-9B3B-B27FFBB9B5B7}"/>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3293376</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1076325</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="59" name="Grafik 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2837B3A5-E745-4362-8C22-F050E6C4F9E7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2741,8 +2744,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="32204025" y="7991475"/>
-          <a:ext cx="3942857" cy="1276190"/>
+          <a:off x="8582025" y="1343025"/>
+          <a:ext cx="3207651" cy="1038225"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2754,22 +2757,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>818657</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>314165</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="57" name="Grafik 56">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{447E6B5B-ACFD-4DA6-9E66-FF0C6A22998E}"/>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>3391471</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1104901</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Grafik 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95B26F3D-FA92-4663-80B2-D0A31F756F6C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2778,42 +2781,42 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId52"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="32356425" y="8143875"/>
-          <a:ext cx="3942857" cy="1276190"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>3293376</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1076325</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="59" name="Grafik 58">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2837B3A5-E745-4362-8C22-F050E6C4F9E7}"/>
+          <a:off x="32232601" y="1323976"/>
+          <a:ext cx="3362895" cy="1085850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>3438385</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="60" name="Grafik 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBA065D6-ACC4-499E-8ABA-BACE251AC7EB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2822,15 +2825,279 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8582025" y="1343025"/>
-          <a:ext cx="3207651" cy="1038225"/>
+          <a:off x="32204026" y="3552825"/>
+          <a:ext cx="3438384" cy="1104900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>3394822</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="62" name="Grafik 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CA4BE94-8E66-4DDA-8D9F-D9EB1CE73716}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId54"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="32251650" y="5772150"/>
+          <a:ext cx="3347197" cy="1104900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>3390900</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1099975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="63" name="Grafik 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2273E26B-F595-426D-B4C2-69E3A8355E75}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="32204025" y="10220325"/>
+          <a:ext cx="3390900" cy="1099975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>47838</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28413</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>3371150</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="64" name="Grafik 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD565751-5164-4771-8AF3-60B928ABE3A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId56"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="32251863" y="218913"/>
+          <a:ext cx="3323312" cy="1105062"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>3438084</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="66" name="Grafik 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A41665AA-2209-481A-A953-8AD237DB971F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId57"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="32232601" y="4714875"/>
+          <a:ext cx="3409508" cy="1057275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>3362326</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>3408219</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="67" name="Grafik 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD3E3E6D-9392-40D6-B670-2B232DE7879F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId58"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="32146876" y="9124951"/>
+          <a:ext cx="3465368" cy="1104900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>3381376</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1087324</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="68" name="Grafik 67">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78AB1943-9B4D-45CC-8525-14142E5A66E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId59"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="32289751" y="2447926"/>
+          <a:ext cx="3295650" cy="1058748"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3142,8 +3409,8 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E3" sqref="E3"/>
+      <pane xSplit="3" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3151,7 +3418,8 @@
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="3" max="10" width="50.7109375" customWidth="1"/>
     <col min="11" max="11" width="51.28515625" customWidth="1"/>
-    <col min="12" max="15" width="24.5703125" customWidth="1"/>
+    <col min="12" max="12" width="51.85546875" customWidth="1"/>
+    <col min="13" max="15" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -3188,7 +3456,9 @@
       <c r="K1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="L1" s="3"/>
+      <c r="L1" s="7" t="s">
+        <v>45</v>
+      </c>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>

</xml_diff>